<commit_message>
Rename "Parent class" to "Parent"
</commit_message>
<xml_diff>
--- a/TSO classes.xlsx
+++ b/TSO classes.xlsx
@@ -1,50 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2">
     <font>
+      <sz val="11.000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
-      <sz val="12"/>
+      <b/>
+      <sz val="12.000000"/>
     </font>
   </fonts>
   <fills count="4">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ebfad0"/>
+        <fgColor rgb="FFEBFAD0"/>
+        <bgColor rgb="FFEBFAD0"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ffffff"/>
+        <fgColor indexed="65"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -58,90 +57,23 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" quotePrefix="0" pivotButton="0"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" quotePrefix="0" pivotButton="0"/>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" quotePrefix="0" pivotButton="0"/>
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" quotePrefix="0" pivotButton="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
@@ -187,13 +119,13 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Thai" typeface="Angsana New"/>
         <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Beng" typeface="Vrinda"/>
         <a:font script="Gujr" typeface="Shruti"/>
@@ -221,13 +153,13 @@
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Thai" typeface="Cordia New"/>
         <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Beng" typeface="Vrinda"/>
         <a:font script="Gujr" typeface="Shruti"/>
@@ -424,13 +356,283 @@
 </a:theme>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,22 +658,22 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Parent class</t>
+          <t xml:space="preserve">Parent class</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Informal definition</t>
+          <t xml:space="preserve">Informal definition</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Logical definition</t>
+          <t xml:space="preserve">Logical definition</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>BFO Entity</t>
+          <t xml:space="preserve">BFO Entity</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -486,7 +688,7 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Entity URL</t>
+          <t xml:space="preserve">Entity URL</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
@@ -501,17 +703,17 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Curation note</t>
+          <t xml:space="preserve">Curation note</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Why fuzzy</t>
+          <t xml:space="preserve">Why fuzzy</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Fuzzy class</t>
+          <t xml:space="preserve">Fuzzy class</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
@@ -521,17 +723,17 @@
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>REL 'tsto:experienceOf'</t>
+          <t xml:space="preserve">REL 'tsto:experienceOf'</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>REL 'owl:equivalentClass'</t>
+          <t xml:space="preserve">REL 'owl:equivalentClass'</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>Curation status</t>
+          <t xml:space="preserve">Curation status</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
@@ -541,15 +743,15 @@
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>Reviewer query</t>
+          <t xml:space="preserve">Reviewer query</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n"/>
+      <c r="A2" s="2"/>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>experience of accident</t>
+          <t xml:space="preserve">experience of accident</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
@@ -559,45 +761,45 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>potentially traumatic experience</t>
+          <t xml:space="preserve">potentially traumatic experience</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>Something that happens which causes potential or actual unintended harm.  Note that DISASTERS are similar but usually impact more people and often (not always) natural forces.</t>
-        </is>
-      </c>
-      <c r="F2" s="2" t="n"/>
-      <c r="G2" s="2" t="n"/>
-      <c r="H2" s="2" t="n"/>
-      <c r="I2" s="2" t="n"/>
-      <c r="J2" s="2" t="n"/>
-      <c r="K2" s="2" t="n"/>
+          <t xml:space="preserve">Something that happens which causes potential or actual unintended harm.  Note that DISASTERS are similar but usually impact more people and often (not always) natural forces.</t>
+        </is>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>includes sub-classes for road traffic accident, fall, animal attack, residential fire, sports-related, weapon-related (unintentional), choking, drowning</t>
-        </is>
-      </c>
-      <c r="M2" s="2" t="n"/>
-      <c r="N2" s="2" t="n"/>
-      <c r="O2" s="2" t="n"/>
+          <t xml:space="preserve">includes sub-classes for road traffic accident, fall, animal attack, residential fire, sports-related, weapon-related (unintentional), choking, drowning</t>
+        </is>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
       <c r="P2" s="2" t="inlineStr">
         <is>
           <t>NKA</t>
         </is>
       </c>
-      <c r="Q2" s="2" t="n"/>
-      <c r="R2" s="2" t="n"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
       <c r="S2" s="2" t="inlineStr">
         <is>
           <t>Pre-proposed</t>
         </is>
       </c>
-      <c r="T2" s="2" t="n"/>
-      <c r="U2" s="2" t="n"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n"/>
+      <c r="A3" s="2"/>
       <c r="B3" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">experience of bereavement </t>
@@ -605,575 +807,575 @@
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>Experience of the death of a loved one</t>
+          <t xml:space="preserve">Experience of the death of a loved one</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>potentially traumatic experience</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="n"/>
-      <c r="F3" s="2" t="n"/>
-      <c r="G3" s="2" t="n"/>
-      <c r="H3" s="2" t="n"/>
-      <c r="I3" s="2" t="n"/>
-      <c r="J3" s="2" t="n"/>
-      <c r="K3" s="2" t="n"/>
+          <t xml:space="preserve">potentially traumatic experience</t>
+        </is>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>need to consult with colleages about sub-classes - probably traumatic bereavement and others</t>
-        </is>
-      </c>
-      <c r="M3" s="2" t="n"/>
-      <c r="N3" s="2" t="n"/>
-      <c r="O3" s="2" t="n"/>
+          <t xml:space="preserve">need to consult with colleages about sub-classes - probably traumatic bereavement and others</t>
+        </is>
+      </c>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
       <c r="P3" s="2" t="inlineStr">
         <is>
           <t>NKA</t>
         </is>
       </c>
-      <c r="Q3" s="2" t="n"/>
-      <c r="R3" s="2" t="n"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
       <c r="S3" s="2" t="inlineStr">
         <is>
           <t>Pre-proposed</t>
         </is>
       </c>
-      <c r="T3" s="2" t="n"/>
-      <c r="U3" s="2" t="n"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="n"/>
+      <c r="A4" s="2"/>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>experience of disaster</t>
+          <t xml:space="preserve">experience of disaster</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>Experience of a sudden-onset occurrence created by natural or technological forces that impacts a group of people defined by place or region</t>
+          <t xml:space="preserve">Experience of a sudden-onset occurrence created by natural or technological forces that impacts a group of people defined by place or region</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>potentially traumatic experience</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="n"/>
-      <c r="F4" s="2" t="n"/>
-      <c r="G4" s="2" t="n"/>
-      <c r="H4" s="2" t="n"/>
-      <c r="I4" s="2" t="n"/>
-      <c r="J4" s="2" t="n"/>
-      <c r="K4" s="2" t="n"/>
+          <t xml:space="preserve">potentially traumatic experience</t>
+        </is>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
       <c r="L4" s="2" t="inlineStr">
         <is>
-          <t>includes sub-classes for natural disaster, technological disaster, transportation disaster (and each of those has multiple sub-classes)</t>
-        </is>
-      </c>
-      <c r="M4" s="2" t="n"/>
-      <c r="N4" s="2" t="n"/>
-      <c r="O4" s="2" t="n"/>
+          <t xml:space="preserve">includes sub-classes for natural disaster, technological disaster, transportation disaster (and each of those has multiple sub-classes)</t>
+        </is>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
       <c r="P4" s="2" t="inlineStr">
         <is>
           <t>NKA</t>
         </is>
       </c>
-      <c r="Q4" s="2" t="n"/>
-      <c r="R4" s="2" t="n"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
       <c r="S4" s="2" t="inlineStr">
         <is>
           <t>Pre-proposed</t>
         </is>
       </c>
-      <c r="T4" s="2" t="n"/>
-      <c r="U4" s="2" t="n"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="n"/>
+      <c r="A5" s="2"/>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>experience of forced labor</t>
+          <t xml:space="preserve">experience of forced labor</t>
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>Experience of being forced to provide labor against one's will</t>
+          <t xml:space="preserve">Experience of being forced to provide labor against one's will</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>potentially traumatic experience</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="n"/>
-      <c r="F5" s="2" t="n"/>
-      <c r="G5" s="2" t="n"/>
-      <c r="H5" s="2" t="n"/>
-      <c r="I5" s="2" t="n"/>
-      <c r="J5" s="2" t="n"/>
-      <c r="K5" s="2" t="n"/>
+          <t xml:space="preserve">potentially traumatic experience</t>
+        </is>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
       <c r="L5" s="2" t="inlineStr">
         <is>
-          <t>includes sub-classes for slavery, human trafficking</t>
-        </is>
-      </c>
-      <c r="M5" s="2" t="n"/>
-      <c r="N5" s="2" t="n"/>
-      <c r="O5" s="2" t="n"/>
+          <t xml:space="preserve">includes sub-classes for slavery, human trafficking</t>
+        </is>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
       <c r="P5" s="2" t="inlineStr">
         <is>
           <t>NKA</t>
         </is>
       </c>
-      <c r="Q5" s="2" t="n"/>
-      <c r="R5" s="2" t="n"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
       <c r="S5" s="2" t="inlineStr">
         <is>
           <t>Pre-proposed</t>
         </is>
       </c>
-      <c r="T5" s="2" t="n"/>
-      <c r="U5" s="2" t="n"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="n"/>
+      <c r="A6" s="2"/>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>experience of health event</t>
+          <t xml:space="preserve">experience of health event</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>Experience of health-related event(s) or treatment</t>
+          <t xml:space="preserve">Experience of health-related event(s) or treatment</t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>potentially traumatic experience</t>
-        </is>
-      </c>
-      <c r="E6" s="2" t="n"/>
-      <c r="F6" s="2" t="n"/>
-      <c r="G6" s="2" t="n"/>
-      <c r="H6" s="2" t="n"/>
-      <c r="I6" s="2" t="n"/>
-      <c r="J6" s="2" t="n"/>
-      <c r="K6" s="2" t="n"/>
+          <t xml:space="preserve">potentially traumatic experience</t>
+        </is>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
       <c r="L6" s="2" t="inlineStr">
         <is>
-          <t>includes sub-classes for injury, illness, treatment experiences (and each of these has sub-classes)</t>
-        </is>
-      </c>
-      <c r="M6" s="2" t="n"/>
-      <c r="N6" s="2" t="n"/>
-      <c r="O6" s="2" t="n"/>
+          <t xml:space="preserve">includes sub-classes for injury, illness, treatment experiences (and each of these has sub-classes)</t>
+        </is>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
       <c r="P6" s="2" t="inlineStr">
         <is>
           <t>NKA</t>
         </is>
       </c>
-      <c r="Q6" s="2" t="n"/>
-      <c r="R6" s="2" t="n"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
       <c r="S6" s="2" t="inlineStr">
         <is>
           <t>Pre-proposed</t>
         </is>
       </c>
-      <c r="T6" s="2" t="n"/>
-      <c r="U6" s="2" t="n"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="n"/>
+      <c r="A7" s="2"/>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>experience of incarceration</t>
+          <t xml:space="preserve">experience of incarceration</t>
         </is>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>Experience of being held against one's will by a government or other state actor</t>
+          <t xml:space="preserve">Experience of being held against one's will by a government or other state actor</t>
         </is>
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>potentially traumatic experience</t>
-        </is>
-      </c>
-      <c r="E7" s="2" t="n"/>
-      <c r="F7" s="2" t="n"/>
-      <c r="G7" s="2" t="n"/>
-      <c r="H7" s="2" t="n"/>
-      <c r="I7" s="2" t="n"/>
-      <c r="J7" s="2" t="n"/>
-      <c r="K7" s="2" t="n"/>
+          <t xml:space="preserve">potentially traumatic experience</t>
+        </is>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
       <c r="L7" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">includes sub-classes for incarceration related to crime, concentration camp imprisonment, political imprisonment, war imprisonment </t>
         </is>
       </c>
-      <c r="M7" s="2" t="n"/>
-      <c r="N7" s="2" t="n"/>
-      <c r="O7" s="2" t="n"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
       <c r="P7" s="2" t="inlineStr">
         <is>
           <t>NKA</t>
         </is>
       </c>
-      <c r="Q7" s="2" t="n"/>
-      <c r="R7" s="2" t="n"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
       <c r="S7" s="2" t="inlineStr">
         <is>
           <t>Pre-proposed</t>
         </is>
       </c>
-      <c r="T7" s="2" t="n"/>
-      <c r="U7" s="2" t="n"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="n"/>
+      <c r="A8" s="2"/>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>experience of interpersonal abuse</t>
+          <t xml:space="preserve">experience of interpersonal abuse</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>Experience of abuse that occurs in a familial or caretaking relationship and that may include physical violence</t>
+          <t xml:space="preserve">Experience of abuse that occurs in a familial or caretaking relationship and that may include physical violence</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>potentially traumatic experience</t>
-        </is>
-      </c>
-      <c r="E8" s="2" t="n"/>
-      <c r="F8" s="2" t="n"/>
-      <c r="G8" s="2" t="n"/>
-      <c r="H8" s="2" t="n"/>
-      <c r="I8" s="2" t="n"/>
-      <c r="J8" s="2" t="n"/>
-      <c r="K8" s="2" t="n"/>
+          <t xml:space="preserve">potentially traumatic experience</t>
+        </is>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
       <c r="L8" s="2" t="inlineStr">
         <is>
-          <t>includes sub-classes: child physical abuse, child sexual abuse, intimate partner violence, elder abuse</t>
-        </is>
-      </c>
-      <c r="M8" s="2" t="n"/>
-      <c r="N8" s="2" t="n"/>
-      <c r="O8" s="2" t="n"/>
+          <t xml:space="preserve">includes sub-classes: child physical abuse, child sexual abuse, intimate partner violence, elder abuse</t>
+        </is>
+      </c>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
       <c r="P8" s="2" t="inlineStr">
         <is>
           <t>NKA</t>
         </is>
       </c>
-      <c r="Q8" s="2" t="n"/>
-      <c r="R8" s="2" t="n"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
       <c r="S8" s="2" t="inlineStr">
         <is>
           <t>Pre-proposed</t>
         </is>
       </c>
-      <c r="T8" s="2" t="n"/>
-      <c r="U8" s="2" t="n"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="n"/>
+      <c r="A9" s="2"/>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>experience of interpersonal violence outside the household</t>
+          <t xml:space="preserve">experience of interpersonal violence outside the household</t>
         </is>
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>Experience of violence directed at an individual by a person outside their household</t>
+          <t xml:space="preserve">Experience of violence directed at an individual by a person outside their household</t>
         </is>
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>potentially traumatic experience</t>
-        </is>
-      </c>
-      <c r="E9" s="2" t="n"/>
-      <c r="F9" s="2" t="n"/>
-      <c r="G9" s="2" t="n"/>
-      <c r="H9" s="2" t="n"/>
-      <c r="I9" s="2" t="n"/>
-      <c r="J9" s="2" t="n"/>
-      <c r="K9" s="2" t="n"/>
+          <t xml:space="preserve">potentially traumatic experience</t>
+        </is>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
       <c r="L9" s="2" t="inlineStr">
         <is>
-          <t>includes sub-classes for physical assault, sexual assault, homicide, abduction-kidnapping, hostage taking, torture</t>
-        </is>
-      </c>
-      <c r="M9" s="2" t="n"/>
-      <c r="N9" s="2" t="n"/>
-      <c r="O9" s="2" t="n"/>
+          <t xml:space="preserve">includes sub-classes for physical assault, sexual assault, homicide, abduction-kidnapping, hostage taking, torture</t>
+        </is>
+      </c>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
       <c r="P9" s="2" t="inlineStr">
         <is>
           <t>NKA</t>
         </is>
       </c>
-      <c r="Q9" s="2" t="n"/>
-      <c r="R9" s="2" t="n"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
       <c r="S9" s="2" t="inlineStr">
         <is>
           <t>Pre-proposed</t>
         </is>
       </c>
-      <c r="T9" s="2" t="n"/>
-      <c r="U9" s="2" t="n"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="n"/>
+      <c r="A10" s="2"/>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>experience of mass violence</t>
+          <t xml:space="preserve">experience of mass violence</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>Experience of violence directed at a group of people</t>
+          <t xml:space="preserve">Experience of violence directed at a group of people</t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>potentially traumatic experience</t>
-        </is>
-      </c>
-      <c r="E10" s="2" t="n"/>
-      <c r="F10" s="2" t="n"/>
-      <c r="G10" s="2" t="n"/>
-      <c r="H10" s="2" t="n"/>
-      <c r="I10" s="2" t="n"/>
-      <c r="J10" s="2" t="n"/>
-      <c r="K10" s="2" t="n"/>
+          <t xml:space="preserve">potentially traumatic experience</t>
+        </is>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
       <c r="L10" s="2" t="inlineStr">
         <is>
-          <t>includes sub-classes for mass injury or homicide, terrorism, genocide</t>
-        </is>
-      </c>
-      <c r="M10" s="2" t="n"/>
-      <c r="N10" s="2" t="n"/>
-      <c r="O10" s="2" t="n"/>
+          <t xml:space="preserve">includes sub-classes for mass injury or homicide, terrorism, genocide</t>
+        </is>
+      </c>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
       <c r="P10" s="2" t="inlineStr">
         <is>
           <t>NKA</t>
         </is>
       </c>
-      <c r="Q10" s="2" t="n"/>
-      <c r="R10" s="2" t="n"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
       <c r="S10" s="2" t="inlineStr">
         <is>
           <t>Pre-proposed</t>
         </is>
       </c>
-      <c r="T10" s="2" t="n"/>
-      <c r="U10" s="2" t="n"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="n"/>
+      <c r="A11" s="2"/>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>experience of migration or displacement</t>
+          <t xml:space="preserve">experience of migration or displacement</t>
         </is>
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>Experience of sudden or forced displacement from one's home or home area because of physical or political danger</t>
+          <t xml:space="preserve">Experience of sudden or forced displacement from one's home or home area because of physical or political danger</t>
         </is>
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>potentially traumatic experience</t>
-        </is>
-      </c>
-      <c r="E11" s="2" t="n"/>
-      <c r="F11" s="2" t="n"/>
-      <c r="G11" s="2" t="n"/>
-      <c r="H11" s="2" t="n"/>
-      <c r="I11" s="2" t="n"/>
-      <c r="J11" s="2" t="n"/>
-      <c r="K11" s="2" t="n"/>
+          <t xml:space="preserve">potentially traumatic experience</t>
+        </is>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
       <c r="L11" s="2" t="inlineStr">
         <is>
-          <t>might include sub-classes for refugee experiences, forced migration, prolonged displacement, climate-related displacement</t>
-        </is>
-      </c>
-      <c r="M11" s="2" t="n"/>
-      <c r="N11" s="2" t="n"/>
-      <c r="O11" s="2" t="n"/>
+          <t xml:space="preserve">might include sub-classes for refugee experiences, forced migration, prolonged displacement, climate-related displacement</t>
+        </is>
+      </c>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
       <c r="P11" s="2" t="inlineStr">
         <is>
           <t>NKA</t>
         </is>
       </c>
-      <c r="Q11" s="2" t="n"/>
-      <c r="R11" s="2" t="n"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
       <c r="S11" s="2" t="inlineStr">
         <is>
           <t>Pre-proposed</t>
         </is>
       </c>
-      <c r="T11" s="2" t="n"/>
-      <c r="U11" s="2" t="n"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="n"/>
+      <c r="A12" s="2"/>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>experience of racial trauma</t>
+          <t xml:space="preserve">experience of racial trauma</t>
         </is>
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>Experience of adverse events related to a person's racial or ethnic identity</t>
+          <t xml:space="preserve">Experience of adverse events related to a person's racial or ethnic identity</t>
         </is>
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
-          <t>potentially traumatic experience</t>
-        </is>
-      </c>
-      <c r="E12" s="2" t="n"/>
-      <c r="F12" s="2" t="n"/>
-      <c r="G12" s="2" t="n"/>
-      <c r="H12" s="2" t="n"/>
-      <c r="I12" s="2" t="n"/>
-      <c r="J12" s="2" t="n"/>
-      <c r="K12" s="2" t="n"/>
+          <t xml:space="preserve">potentially traumatic experience</t>
+        </is>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
       <c r="L12" s="2" t="inlineStr">
         <is>
-          <t>includes sub-classes for experiences of racism, hate crimes, micro-agressions, generational trauma</t>
-        </is>
-      </c>
-      <c r="M12" s="2" t="n"/>
-      <c r="N12" s="2" t="n"/>
-      <c r="O12" s="2" t="n"/>
+          <t xml:space="preserve">includes sub-classes for experiences of racism, hate crimes, micro-agressions, generational trauma</t>
+        </is>
+      </c>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
       <c r="P12" s="2" t="inlineStr">
         <is>
           <t>NKA</t>
         </is>
       </c>
-      <c r="Q12" s="2" t="n"/>
-      <c r="R12" s="2" t="n"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
       <c r="S12" s="2" t="inlineStr">
         <is>
           <t>Pre-proposed</t>
         </is>
       </c>
-      <c r="T12" s="2" t="n"/>
-      <c r="U12" s="2" t="n"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="n"/>
+      <c r="A13" s="2"/>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>experience of violent social environment</t>
+          <t xml:space="preserve">experience of violent social environment</t>
         </is>
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>Experience of being exposed to violence or threatened violence in the social and physical environment outside the household</t>
+          <t xml:space="preserve">Experience of being exposed to violence or threatened violence in the social and physical environment outside the household</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>potentially traumatic experience</t>
-        </is>
-      </c>
-      <c r="E13" s="2" t="n"/>
-      <c r="F13" s="2" t="n"/>
-      <c r="G13" s="2" t="n"/>
-      <c r="H13" s="2" t="n"/>
-      <c r="I13" s="2" t="n"/>
-      <c r="J13" s="2" t="n"/>
-      <c r="K13" s="2" t="n"/>
+          <t xml:space="preserve">potentially traumatic experience</t>
+        </is>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
       <c r="L13" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">includes sub-classes for community evironment of violence; school enviroment of violence; workplace enviroment of violence; environment of violence related to gender, ethnicity or other marginalized identity  </t>
         </is>
       </c>
-      <c r="M13" s="2" t="n"/>
-      <c r="N13" s="2" t="n"/>
-      <c r="O13" s="2" t="n"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
       <c r="P13" s="2" t="inlineStr">
         <is>
           <t>NKA</t>
         </is>
       </c>
-      <c r="Q13" s="2" t="n"/>
-      <c r="R13" s="2" t="n"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
       <c r="S13" s="2" t="inlineStr">
         <is>
           <t>Pre-proposed</t>
         </is>
       </c>
-      <c r="T13" s="2" t="n"/>
-      <c r="U13" s="2" t="n"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="n"/>
+      <c r="A14" s="2"/>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>experience of war or armed conflict</t>
+          <t xml:space="preserve">experience of war or armed conflict</t>
         </is>
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>Experience of armed conflict between states or other military groups</t>
+          <t xml:space="preserve">Experience of armed conflict between states or other military groups</t>
         </is>
       </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
-          <t>potentially traumatic experience</t>
-        </is>
-      </c>
-      <c r="E14" s="2" t="n"/>
-      <c r="F14" s="2" t="n"/>
-      <c r="G14" s="2" t="n"/>
-      <c r="H14" s="2" t="n"/>
-      <c r="I14" s="2" t="n"/>
-      <c r="J14" s="2" t="n"/>
-      <c r="K14" s="2" t="n"/>
+          <t xml:space="preserve">potentially traumatic experience</t>
+        </is>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>includes sub-classes for civilian exposure to warfare or armed conflict, combat exposure as a member of armed forces, deployment as a member of armed forces</t>
-        </is>
-      </c>
-      <c r="M14" s="2" t="n"/>
-      <c r="N14" s="2" t="n"/>
-      <c r="O14" s="2" t="n"/>
+          <t xml:space="preserve">includes sub-classes for civilian exposure to warfare or armed conflict, combat exposure as a member of armed forces, deployment as a member of armed forces</t>
+        </is>
+      </c>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
       <c r="P14" s="2" t="inlineStr">
         <is>
           <t>NKA</t>
         </is>
       </c>
-      <c r="Q14" s="2" t="n"/>
-      <c r="R14" s="2" t="n"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
       <c r="S14" s="2" t="inlineStr">
         <is>
           <t>Pre-proposed</t>
         </is>
       </c>
-      <c r="T14" s="2" t="n"/>
-      <c r="U14" s="2" t="n"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
     </row>
     <row r="15">
       <c r="B15" t="inlineStr">
         <is>
-          <t>nature of exposure to potentially traumatic experience</t>
+          <t xml:space="preserve">nature of exposure to potentially traumatic experience</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>An attribute of a potentially traumatic experience that is the nature of a person's exposure (ie, direct vs indirect)</t>
+          <t xml:space="preserve">An attribute of a potentially traumatic experience that is the nature of a person's exposure (ie, direct vs indirect)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>potentially traumatic experience attribute</t>
+          <t xml:space="preserve">potentially traumatic experience attribute</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -1190,12 +1392,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>personal history</t>
+          <t xml:space="preserve">personal history</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>A history that is of a person.</t>
+          <t xml:space="preserve">A history that is of a person.</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1205,12 +1407,12 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>The whole of someone's life story including what they do and what happens to them.</t>
+          <t xml:space="preserve">The whole of someone's life story including what they do and what happens to them.</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>experienced event; exposure</t>
+          <t xml:space="preserve">experienced event; exposure</t>
         </is>
       </c>
     </row>
@@ -1222,12 +1424,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>personal history part</t>
+          <t xml:space="preserve">personal history part</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>A process that is part of a personal history.</t>
+          <t xml:space="preserve">A process that is part of a personal history.</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1237,61 +1439,61 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>A part of a person's life story.</t>
+          <t xml:space="preserve">A part of a person's life story.</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>trauma exposure</t>
+          <t xml:space="preserve">trauma exposure</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="inlineStr"/>
+      <c r="A18" s="3"/>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>potentially traumatic experience</t>
+          <t xml:space="preserve">potentially traumatic experience</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>A personal history part that may lead to traumatic stress responses</t>
+          <t xml:space="preserve">A personal history part that may lead to traumatic stress responses</t>
         </is>
       </c>
       <c r="D18" s="3" t="inlineStr">
         <is>
-          <t>personal history part</t>
-        </is>
-      </c>
-      <c r="E18" s="3" t="n"/>
-      <c r="F18" s="3" t="n"/>
-      <c r="G18" s="3" t="n"/>
-      <c r="H18" s="3" t="n"/>
-      <c r="I18" s="3" t="n"/>
-      <c r="J18" s="3" t="n"/>
-      <c r="K18" s="3" t="n"/>
+          <t xml:space="preserve">personal history part</t>
+        </is>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
       <c r="L18" s="3" t="inlineStr">
         <is>
-          <t>There is lots of debate in the field about how and whether to define a class of events that are potentially traumatic.  Given that debate, I think best to state something along these lines.</t>
-        </is>
-      </c>
-      <c r="M18" s="3" t="n"/>
-      <c r="N18" s="3" t="n"/>
-      <c r="O18" s="3" t="n"/>
+          <t xml:space="preserve">There is lots of debate in the field about how and whether to define a class of events that are potentially traumatic.  Given that debate, I think best to state something along these lines.</t>
+        </is>
+      </c>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
       <c r="P18" s="3" t="inlineStr">
         <is>
           <t>NKA</t>
         </is>
       </c>
-      <c r="Q18" s="3" t="n"/>
-      <c r="R18" s="3" t="n"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
       <c r="S18" s="3" t="inlineStr">
         <is>
           <t>Proposed</t>
         </is>
       </c>
-      <c r="T18" s="3" t="n"/>
-      <c r="U18" s="3" t="n"/>
+      <c r="T18" s="3"/>
+      <c r="U18" s="3"/>
     </row>
     <row r="19">
       <c r="B19" t="inlineStr">
@@ -1301,12 +1503,12 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>An attribute of a potentially traumatic experience that is the degree of human agency involved in causing the event(s) experienced</t>
+          <t xml:space="preserve">An attribute of a potentially traumatic experience that is the degree of human agency involved in causing the event(s) experienced</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>potentially traumatic experience attribute</t>
+          <t xml:space="preserve">potentially traumatic experience attribute</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1321,10 +1523,10 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="2" t="n"/>
+      <c r="A20" s="2"/>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>potentially traumatic experience attribute</t>
+          <t xml:space="preserve">potentially traumatic experience attribute</t>
         </is>
       </c>
       <c r="C20" s="2" t="inlineStr">
@@ -1339,48 +1541,48 @@
       </c>
       <c r="E20" s="2" t="inlineStr">
         <is>
-          <t>Attributes of PTEs include their type, time course, severity, degree of human agency involved in the event, nature of exposure (direct vs indirect)</t>
-        </is>
-      </c>
-      <c r="F20" s="2" t="n"/>
-      <c r="G20" s="2" t="n"/>
-      <c r="H20" s="2" t="n"/>
-      <c r="I20" s="2" t="n"/>
-      <c r="J20" s="2" t="n"/>
-      <c r="K20" s="2" t="n"/>
-      <c r="L20" s="2" t="n"/>
-      <c r="M20" s="2" t="n"/>
-      <c r="N20" s="2" t="n"/>
-      <c r="O20" s="2" t="n"/>
+          <t xml:space="preserve">Attributes of PTEs include their type, time course, severity, degree of human agency involved in the event, nature of exposure (direct vs indirect)</t>
+        </is>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
       <c r="P20" s="2" t="inlineStr">
         <is>
           <t>NKA</t>
         </is>
       </c>
-      <c r="Q20" s="2" t="n"/>
-      <c r="R20" s="2" t="n"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
       <c r="S20" s="2" t="inlineStr">
         <is>
           <t>Pre-proposed</t>
         </is>
       </c>
-      <c r="T20" s="2" t="n"/>
-      <c r="U20" s="2" t="n"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
     </row>
     <row r="21">
       <c r="B21" t="inlineStr">
         <is>
-          <t>potentially traumatic experience severity</t>
+          <t xml:space="preserve">potentially traumatic experience severity</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>An attribute of a potentially traumatic experience that is the severity of the event(s) experienced</t>
+          <t xml:space="preserve">An attribute of a potentially traumatic experience that is the severity of the event(s) experienced</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>potentially traumatic experience attribute</t>
+          <t xml:space="preserve">potentially traumatic experience attribute</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1390,7 +1592,7 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Severity might be seen as a combination of several other attributes listed here - but I think we often think of this as an independent dimension.  Should there be sub-classes for obective severity and subjective or perceived severity, or for objective and perceived life threat?   - to be discussed with colleagues</t>
+          <t xml:space="preserve">Severity might be seen as a combination of several other attributes listed here - but I think we often think of this as an independent dimension.  Should there be sub-classes for obective severity and subjective or perceived severity, or for objective and perceived life threat?   - to be discussed with colleagues</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -1402,22 +1604,22 @@
     <row r="22">
       <c r="B22" t="inlineStr">
         <is>
-          <t>potentially traumatic experience time course</t>
+          <t xml:space="preserve">potentially traumatic experience time course</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>An attribute of a potentially traumatic experience that is its chronicity</t>
+          <t xml:space="preserve">An attribute of a potentially traumatic experience that is its chronicity</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>potentially traumatic experience attribute</t>
+          <t xml:space="preserve">potentially traumatic experience attribute</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>include sub-classes for chronicity, frequency, duration, age at onset</t>
+          <t xml:space="preserve">include sub-classes for chronicity, frequency, duration, age at onset</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -1429,22 +1631,22 @@
     <row r="23">
       <c r="B23" t="inlineStr">
         <is>
-          <t>potentially traumatic experience type</t>
+          <t xml:space="preserve">potentially traumatic experience type</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>An attribute of a potentially traumatic experience that is the type of event(s) experienced by a person</t>
+          <t xml:space="preserve">An attribute of a potentially traumatic experience that is the type of event(s) experienced by a person</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>potentially traumatic experience attribute</t>
+          <t xml:space="preserve">potentially traumatic experience attribute</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>event type</t>
+          <t xml:space="preserve">event type</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -1466,7 +1668,7 @@
       </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
-          <t>An occurrent that has temporal proper parts and for some time t.</t>
+          <t xml:space="preserve">An occurrent that has temporal proper parts and for some time t.</t>
         </is>
       </c>
       <c r="D24" s="2" t="inlineStr">
@@ -1476,29 +1678,29 @@
       </c>
       <c r="E24" s="2" t="inlineStr">
         <is>
-          <t>Something that happens over time and involves some kind of change.</t>
-        </is>
-      </c>
-      <c r="F24" s="2" t="n"/>
-      <c r="G24" s="2" t="n"/>
-      <c r="H24" s="2" t="n"/>
-      <c r="I24" s="2" t="n"/>
-      <c r="J24" s="2" t="n"/>
-      <c r="K24" s="2" t="n"/>
-      <c r="L24" s="2" t="n"/>
-      <c r="M24" s="2" t="n"/>
-      <c r="N24" s="2" t="n"/>
-      <c r="O24" s="2" t="n"/>
-      <c r="P24" s="2" t="n"/>
-      <c r="Q24" s="2" t="n"/>
-      <c r="R24" s="2" t="n"/>
+          <t xml:space="preserve">Something that happens over time and involves some kind of change.</t>
+        </is>
+      </c>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
       <c r="S24" s="2" t="inlineStr">
         <is>
           <t>Pre-proposed</t>
         </is>
       </c>
-      <c r="T24" s="2" t="n"/>
-      <c r="U24" s="2" t="n"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>